<commit_message>
fixing tag location import
</commit_message>
<xml_diff>
--- a/public/download/location.xlsx
+++ b/public/download/location.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbookpro/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/logsheet_php/public/download/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{978D9D11-1A04-B140-855F-764591DDEE81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC8A7BB-76BC-734F-A7DA-5CDC5ED12665}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="440" windowWidth="25440" windowHeight="14580" xr2:uid="{79730054-C2F2-A84A-8F4C-D42923722402}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>#</t>
   </si>
@@ -82,6 +82,30 @@
   </si>
   <si>
     <t>longitude</t>
+  </si>
+  <si>
+    <t>Location 8</t>
+  </si>
+  <si>
+    <t>Location 9</t>
+  </si>
+  <si>
+    <t>Location 10</t>
+  </si>
+  <si>
+    <t>Location 11</t>
+  </si>
+  <si>
+    <t>desc 8</t>
+  </si>
+  <si>
+    <t>desc 9</t>
+  </si>
+  <si>
+    <t>desc 10</t>
+  </si>
+  <si>
+    <t>desc 11</t>
   </si>
 </sst>
 </file>
@@ -103,15 +127,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -119,12 +149,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,148 +490,223 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D52F97D0-388F-2649-AD7A-C936E029A901}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E2" sqref="E2:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.83203125" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:5" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>